<commit_message>
Changed few components to do manufacturing possible.
</commit_message>
<xml_diff>
--- a/cam/Uno_v1.0_2021-05-02-PnP.xlsx
+++ b/cam/Uno_v1.0_2021-05-02-PnP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\Uno\cam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\UNO-328\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6C7EB6-81E6-43FF-8E04-518B0DAFB1ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03EF5159-F6CE-4EAB-87D4-CABCBB8C6087}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24420" yWindow="830" windowWidth="16430" windowHeight="19950" xr2:uid="{C9210FEF-8F38-4EDD-9F73-37179BB1DAE7}"/>
+    <workbookView xWindow="3040" yWindow="1650" windowWidth="16430" windowHeight="19950" xr2:uid="{C9210FEF-8F38-4EDD-9F73-37179BB1DAE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -610,7 +610,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,7 +991,7 @@
         <v>58</v>
       </c>
       <c r="E22" s="1">
-        <v>270</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>